<commit_message>
ran code with no addons
</commit_message>
<xml_diff>
--- a/results/11-2020/fim_interactive.xlsx
+++ b/results/11-2020/fim_interactive.xlsx
@@ -422,10 +422,10 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>-0.04873127066753441</v>
+        <v>-0.04932278832823928</v>
       </c>
       <c r="F2">
-        <v>-0.4472294074885929</v>
+        <v>-0.4469858474916468</v>
       </c>
       <c r="G2">
         <v>0.2318136940835876</v>
@@ -434,7 +434,7 @@
         <v>0.1384476835461522</v>
       </c>
       <c r="I2">
-        <v>-0.4189926482972742</v>
+        <v>-0.419584165957979</v>
       </c>
     </row>
     <row r="3">
@@ -455,19 +455,19 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>-1.88755655971204</v>
+        <v>-1.889666396925633</v>
       </c>
       <c r="F3">
-        <v>-0.7456669684567119</v>
+        <v>-0.7463849117283146</v>
       </c>
       <c r="G3">
         <v>-1.31159166141865</v>
       </c>
       <c r="H3">
-        <v>0.03883989562439164</v>
+        <v>0.03883989562439163</v>
       </c>
       <c r="I3">
-        <v>-0.6148047939177821</v>
+        <v>-0.6169146311313748</v>
       </c>
     </row>
     <row r="4">
@@ -488,10 +488,10 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>-0.3090944267481067</v>
+        <v>-0.3089450243958607</v>
       </c>
       <c r="F4">
-        <v>-0.6103231932502594</v>
+        <v>-0.6109690798429839</v>
       </c>
       <c r="G4">
         <v>0.4707108944060808</v>
@@ -500,7 +500,7 @@
         <v>-0.5107329829851925</v>
       </c>
       <c r="I4">
-        <v>-0.2690723381689949</v>
+        <v>-0.268922935816749</v>
       </c>
     </row>
     <row r="5">
@@ -521,19 +521,19 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>-1.107555438830284</v>
+        <v>-1.107596038569778</v>
       </c>
       <c r="F5">
-        <v>-0.8382344239894907</v>
+        <v>-0.8388825620548781</v>
       </c>
       <c r="G5">
         <v>-0.7542304097927617</v>
       </c>
       <c r="H5">
-        <v>-0.2606953291135497</v>
+        <v>-0.2606953291135496</v>
       </c>
       <c r="I5">
-        <v>-0.09262969992397241</v>
+        <v>-0.09267029966346674</v>
       </c>
     </row>
     <row r="6">
@@ -554,10 +554,10 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>-0.2185905956505214</v>
+        <v>-0.2174362895015348</v>
       </c>
       <c r="F6">
-        <v>-0.8806992552352374</v>
+        <v>-0.880910937348202</v>
       </c>
       <c r="G6">
         <v>0.03794677656077419</v>
@@ -566,7 +566,7 @@
         <v>-0.2790588276696364</v>
       </c>
       <c r="I6">
-        <v>0.02252145545834081</v>
+        <v>0.02367576160732738</v>
       </c>
     </row>
     <row r="7">
@@ -587,10 +587,10 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0.6910360014545981</v>
+        <v>0.6916906192687385</v>
       </c>
       <c r="F7">
-        <v>-0.2360511149435778</v>
+        <v>-0.2355716832996092</v>
       </c>
       <c r="G7">
         <v>0.4176699769362638</v>
@@ -599,7 +599,7 @@
         <v>0.03463379122030326</v>
       </c>
       <c r="I7">
-        <v>0.238732233298031</v>
+        <v>0.2393868511121715</v>
       </c>
     </row>
     <row r="8">
@@ -620,10 +620,10 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1.027385345497273</v>
+        <v>1.028743299593723</v>
       </c>
       <c r="F8">
-        <v>0.0980688281177672</v>
+        <v>0.09885039769778682</v>
       </c>
       <c r="G8">
         <v>0.3854233068740954</v>
@@ -632,7 +632,7 @@
         <v>0.2634165840868962</v>
       </c>
       <c r="I8">
-        <v>0.3785454545362815</v>
+        <v>0.3799034086327318</v>
       </c>
     </row>
     <row r="9">
@@ -653,10 +653,10 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0.801022958330558</v>
+        <v>0.8009557549500425</v>
       </c>
       <c r="F9">
-        <v>0.5752134274079777</v>
+        <v>0.575988346077742</v>
       </c>
       <c r="G9">
         <v>-0.3246051547334287</v>
@@ -665,7 +665,7 @@
         <v>-0.3447600652268802</v>
       </c>
       <c r="I9">
-        <v>1.470388178290867</v>
+        <v>1.470320974910351</v>
       </c>
     </row>
     <row r="10">
@@ -686,10 +686,10 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>1.92051494273168</v>
+        <v>1.919839734374504</v>
       </c>
       <c r="F10">
-        <v>1.109989812003528</v>
+        <v>1.110307352046752</v>
       </c>
       <c r="G10">
         <v>0.1230989010896827</v>
@@ -698,7 +698,7 @@
         <v>0.5335658662608733</v>
       </c>
       <c r="I10">
-        <v>1.263850175381124</v>
+        <v>1.263174967023948</v>
       </c>
     </row>
     <row r="11">
@@ -719,10 +719,10 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>2.285535806575335</v>
+        <v>2.285342222525221</v>
       </c>
       <c r="F11">
-        <v>1.508614763283712</v>
+        <v>1.508720252860872</v>
       </c>
       <c r="G11">
         <v>1.052245127335171</v>
@@ -731,7 +731,7 @@
         <v>-0.2965791441100969</v>
       </c>
       <c r="I11">
-        <v>1.529869823350261</v>
+        <v>1.529676239300148</v>
       </c>
     </row>
     <row r="12">
@@ -752,10 +752,10 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1.931644997024508</v>
+        <v>1.931965411866221</v>
       </c>
       <c r="F12">
-        <v>1.734679676165521</v>
+        <v>1.734525780928997</v>
       </c>
       <c r="G12">
         <v>0.3185676646894323</v>
@@ -764,7 +764,7 @@
         <v>-0.2595992058963156</v>
       </c>
       <c r="I12">
-        <v>1.872676538231392</v>
+        <v>1.872996953073104</v>
       </c>
     </row>
     <row r="13">
@@ -785,10 +785,10 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>1.443739216222842</v>
+        <v>1.443771624297853</v>
       </c>
       <c r="F13">
-        <v>1.895358740638592</v>
+        <v>1.895229748265949</v>
       </c>
       <c r="G13">
         <v>-0.08532620047935681</v>
@@ -797,7 +797,7 @@
         <v>-0.02386484856737564</v>
       </c>
       <c r="I13">
-        <v>1.552930265269575</v>
+        <v>1.552962673344586</v>
       </c>
     </row>
     <row r="14">
@@ -818,19 +818,19 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>1.187712274604291</v>
+        <v>1.188166172820331</v>
       </c>
       <c r="F14">
-        <v>1.712158073606745</v>
+        <v>1.712311357877406</v>
       </c>
       <c r="G14">
         <v>0.3456853209154376</v>
       </c>
       <c r="H14">
-        <v>-0.2574736546801013</v>
+        <v>-0.2574736546801012</v>
       </c>
       <c r="I14">
-        <v>1.099500608368954</v>
+        <v>1.099954506584995</v>
       </c>
     </row>
     <row r="15">
@@ -851,10 +851,10 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0.7133263378476467</v>
+        <v>0.7128131158019653</v>
       </c>
       <c r="F15">
-        <v>1.319105706424823</v>
+        <v>1.319179081196592</v>
       </c>
       <c r="G15">
         <v>0.0406776650144408</v>
@@ -863,7 +863,7 @@
         <v>-0.4619483423637046</v>
       </c>
       <c r="I15">
-        <v>1.134597015196911</v>
+        <v>1.134083793151229</v>
       </c>
     </row>
     <row r="16">
@@ -884,10 +884,10 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1.385299507138876</v>
+        <v>1.38384912093355</v>
       </c>
       <c r="F16">
-        <v>1.182519333953415</v>
+        <v>1.182150008463424</v>
       </c>
       <c r="G16">
         <v>1.665594538201976</v>
@@ -896,7 +896,7 @@
         <v>-1.43490081457891</v>
       </c>
       <c r="I16">
-        <v>1.154605783515809</v>
+        <v>1.153155397310484</v>
       </c>
     </row>
     <row r="17">
@@ -917,10 +917,10 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0.5884807197534302</v>
+        <v>0.5882778225287952</v>
       </c>
       <c r="F17">
-        <v>0.9687047098360617</v>
+        <v>0.9682765580211596</v>
       </c>
       <c r="G17">
         <v>-0.7323423591140148</v>
@@ -929,7 +929,7 @@
         <v>0.3998565275949437</v>
       </c>
       <c r="I17">
-        <v>0.9209665512725013</v>
+        <v>0.9207636540478663</v>
       </c>
     </row>
     <row r="18">
@@ -950,10 +950,10 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>0.6483471362496426</v>
+        <v>0.6484157767578571</v>
       </c>
       <c r="F18">
-        <v>0.8338634252473998</v>
+        <v>0.8333389590055411</v>
       </c>
       <c r="G18">
         <v>0.5092651698143085</v>
@@ -962,7 +962,7 @@
         <v>-0.546989131172936</v>
       </c>
       <c r="I18">
-        <v>0.6860710976082701</v>
+        <v>0.6861397381164847</v>
       </c>
     </row>
     <row r="19">
@@ -983,19 +983,19 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>0.07706421107389419</v>
+        <v>0.07736815158605984</v>
       </c>
       <c r="F19">
-        <v>0.6747978935539617</v>
+        <v>0.6744777179515649</v>
       </c>
       <c r="G19">
-        <v>-0.4041200882597879</v>
+        <v>-0.4041200882597878</v>
       </c>
       <c r="H19">
         <v>0.2335694975294421</v>
       </c>
       <c r="I19">
-        <v>0.24761480180424</v>
+        <v>0.2479187423164056</v>
       </c>
     </row>
     <row r="20">
@@ -1016,10 +1016,10 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>-0.1197440912471906</v>
+        <v>-0.1204265298871156</v>
       </c>
       <c r="F20">
-        <v>0.2985369939574451</v>
+        <v>0.2984088052463984</v>
       </c>
       <c r="G20">
         <v>-0.2813714609987538</v>
@@ -1028,7 +1028,7 @@
         <v>-0.03567393639946731</v>
       </c>
       <c r="I20">
-        <v>0.1973013061510305</v>
+        <v>0.1966188675111055</v>
       </c>
     </row>
     <row r="21">
@@ -1049,10 +1049,10 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>-0.4654912699649514</v>
+        <v>-0.4655468536569111</v>
       </c>
       <c r="F21">
-        <v>0.0350439965278497</v>
+        <v>0.03495263619997183</v>
       </c>
       <c r="G21">
         <v>0.3398770253391276</v>
@@ -1061,7 +1061,7 @@
         <v>-0.7314416061911453</v>
       </c>
       <c r="I21">
-        <v>-0.07392668911293369</v>
+        <v>-0.07398227280489336</v>
       </c>
     </row>
     <row r="22">
@@ -1082,10 +1082,10 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>-0.6667320013633891</v>
+        <v>-0.66597156096414</v>
       </c>
       <c r="F22">
-        <v>-0.2937257878754082</v>
+        <v>-0.2936441982305275</v>
       </c>
       <c r="G22">
         <v>-0.3550314415416719</v>
@@ -1094,7 +1094,7 @@
         <v>-0.2307444377000993</v>
       </c>
       <c r="I22">
-        <v>-0.080956122121618</v>
+        <v>-0.08019568172236891</v>
       </c>
     </row>
     <row r="23">
@@ -1115,10 +1115,10 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>-0.6360786025057481</v>
+        <v>-0.6363277001230021</v>
       </c>
       <c r="F23">
-        <v>-0.4720114912703188</v>
+        <v>-0.4720681611577929</v>
       </c>
       <c r="G23">
         <v>0.02168388493087975</v>
@@ -1127,7 +1127,7 @@
         <v>-0.1581741428903265</v>
       </c>
       <c r="I23">
-        <v>-0.4995883445463014</v>
+        <v>-0.4998374421635554</v>
       </c>
     </row>
     <row r="24">
@@ -1148,10 +1148,10 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>-1.059035740127722</v>
+        <v>-1.059191424855756</v>
       </c>
       <c r="F24">
-        <v>-0.7068344034904516</v>
+        <v>-0.7067593848999529</v>
       </c>
       <c r="G24">
         <v>-0.2701579859382386</v>
@@ -1160,7 +1160,7 @@
         <v>-0.2764818884085525</v>
       </c>
       <c r="I24">
-        <v>-0.5123958657809304</v>
+        <v>-0.5125515505089645</v>
       </c>
     </row>
     <row r="25">
@@ -1181,10 +1181,10 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>-0.7633323808550926</v>
+        <v>-0.7625094549814095</v>
       </c>
       <c r="F25">
-        <v>-0.7812946812129868</v>
+        <v>-0.7810000352310775</v>
       </c>
       <c r="G25">
         <v>-0.1071728628412014</v>
@@ -1193,7 +1193,7 @@
         <v>-0.1249180002665537</v>
       </c>
       <c r="I25">
-        <v>-0.5312415177473375</v>
+        <v>-0.5304185918736545</v>
       </c>
     </row>
     <row r="26">
@@ -1214,10 +1214,10 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>-0.868496698635547</v>
+        <v>-0.8686373311051071</v>
       </c>
       <c r="F26">
-        <v>-0.8317358555310264</v>
+        <v>-0.8316664777663193</v>
       </c>
       <c r="G26">
         <v>-0.2767950136222138</v>
@@ -1226,7 +1226,7 @@
         <v>-0.1302645945694583</v>
       </c>
       <c r="I26">
-        <v>-0.4614370904438749</v>
+        <v>-0.461577722913435</v>
       </c>
     </row>
     <row r="27">
@@ -1247,10 +1247,10 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>-0.08904151706259766</v>
+        <v>-0.08933197463653653</v>
       </c>
       <c r="F27">
-        <v>-0.6949765841702387</v>
+        <v>-0.6949175463947028</v>
       </c>
       <c r="G27">
         <v>0.6877869103813896</v>
@@ -1259,7 +1259,7 @@
         <v>-0.1683661652429188</v>
       </c>
       <c r="I27">
-        <v>-0.6084622622010686</v>
+        <v>-0.6087527197750074</v>
       </c>
     </row>
     <row r="28">
@@ -1280,10 +1280,10 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>-1.121428329652999</v>
+        <v>-1.121362038847531</v>
       </c>
       <c r="F28">
-        <v>-0.710574731551558</v>
+        <v>-0.7104601998926466</v>
       </c>
       <c r="G28">
         <v>-0.4905032062218124</v>
@@ -1292,7 +1292,7 @@
         <v>0.03320395040116637</v>
       </c>
       <c r="I28">
-        <v>-0.6641290738323532</v>
+        <v>-0.664062783026885</v>
       </c>
     </row>
     <row r="29">
@@ -1313,10 +1313,10 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>-0.8023196183270442</v>
+        <v>-0.8025841134312768</v>
       </c>
       <c r="F29">
-        <v>-0.720321540919546</v>
+        <v>-0.7204788645051134</v>
       </c>
       <c r="G29">
         <v>-0.6627889888787315</v>
@@ -1325,7 +1325,7 @@
         <v>0.1395514339167008</v>
       </c>
       <c r="I29">
-        <v>-0.2790820633650136</v>
+        <v>-0.2793465584692461</v>
       </c>
     </row>
     <row r="30">
@@ -1346,10 +1346,10 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>-0.04565329217308461</v>
+        <v>-0.04497306661156075</v>
       </c>
       <c r="F30">
-        <v>-0.5146106893039304</v>
+        <v>-0.5145627983817269</v>
       </c>
       <c r="G30">
         <v>0.0405326156052338</v>
@@ -1358,7 +1358,7 @@
         <v>0.202729765204821</v>
       </c>
       <c r="I30">
-        <v>-0.2889156729831394</v>
+        <v>-0.2882354474216156</v>
       </c>
     </row>
     <row r="31">
@@ -1379,10 +1379,10 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>-0.5940432398129916</v>
+        <v>-0.5945145374658474</v>
       </c>
       <c r="F31">
-        <v>-0.640861119991529</v>
+        <v>-0.6408584390890546</v>
       </c>
       <c r="G31">
         <v>-0.4482138378535143</v>
@@ -1391,7 +1391,7 @@
         <v>0.1914173671366676</v>
       </c>
       <c r="I31">
-        <v>-0.3372467690961448</v>
+        <v>-0.3377180667490006</v>
       </c>
     </row>
     <row r="32">
@@ -1412,10 +1412,10 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>0.04940884206564261</v>
+        <v>0.04949840875269429</v>
       </c>
       <c r="F32">
-        <v>-0.3481518270618685</v>
+        <v>-0.3481433271889983</v>
       </c>
       <c r="G32">
         <v>0.6845768143843559</v>
@@ -1424,7 +1424,7 @@
         <v>-0.3565550164851028</v>
       </c>
       <c r="I32">
-        <v>-0.2786129558336105</v>
+        <v>-0.2785233891465588</v>
       </c>
     </row>
     <row r="33">
@@ -1445,10 +1445,10 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>-0.06787364306475245</v>
+        <v>-0.06747215153773298</v>
       </c>
       <c r="F33">
-        <v>-0.1645403332462955</v>
+        <v>-0.1643653367156124</v>
       </c>
       <c r="G33">
         <v>-0.08640542978502515</v>
@@ -1457,7 +1457,7 @@
         <v>0.06632580721215653</v>
       </c>
       <c r="I33">
-        <v>-0.04779402049188383</v>
+        <v>-0.04739252896486435</v>
       </c>
     </row>
     <row r="34">
@@ -1478,10 +1478,10 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>0.2930068653878942</v>
+        <v>0.2925968720771208</v>
       </c>
       <c r="F34">
-        <v>-0.07987529385605083</v>
+        <v>-0.07997285204344198</v>
       </c>
       <c r="G34">
         <v>0.134181683212793</v>
@@ -1490,7 +1490,7 @@
         <v>0.1080155521227334</v>
       </c>
       <c r="I34">
-        <v>0.05080963005236774</v>
+        <v>0.05039963674159439</v>
       </c>
     </row>
     <row r="35">
@@ -1511,10 +1511,10 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>-0.05500495643226036</v>
+        <v>-0.05470159743612268</v>
       </c>
       <c r="F35">
-        <v>0.05488427698913198</v>
+        <v>0.05498038296398919</v>
       </c>
       <c r="G35">
         <v>0.3175547462742406</v>
@@ -1523,7 +1523,7 @@
         <v>-0.5011733566315455</v>
       </c>
       <c r="I35">
-        <v>0.1286136539250445</v>
+        <v>0.1289170129211822</v>
       </c>
     </row>
     <row r="36">
@@ -1544,10 +1544,10 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>2.604355249890733</v>
+        <v>2.604105573262943</v>
       </c>
       <c r="F36">
-        <v>0.6936208789454045</v>
+        <v>0.6936321740915514</v>
       </c>
       <c r="G36">
         <v>0.5310600703908137</v>
@@ -1556,7 +1556,7 @@
         <v>-0.1974623965262828</v>
       </c>
       <c r="I36">
-        <v>2.270757576026202</v>
+        <v>2.270507899398412</v>
       </c>
     </row>
     <row r="37">
@@ -1577,10 +1577,10 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>1.413474371904715</v>
+        <v>1.412453084073397</v>
       </c>
       <c r="F37">
-        <v>1.063957882687771</v>
+        <v>1.063613482994334</v>
       </c>
       <c r="G37">
         <v>-0.002758138597635018</v>
@@ -1589,7 +1589,7 @@
         <v>0.3093434144177715</v>
       </c>
       <c r="I37">
-        <v>1.106889096084578</v>
+        <v>1.105867808253261</v>
       </c>
     </row>
     <row r="38">
@@ -1610,10 +1610,10 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <v>1.632737114848934</v>
+        <v>1.633001091925851</v>
       </c>
       <c r="F38">
-        <v>1.398890445053031</v>
+        <v>1.398714537956517</v>
       </c>
       <c r="G38">
         <v>0.5136971469729917</v>
@@ -1622,7 +1622,7 @@
         <v>-0.2960053567725832</v>
       </c>
       <c r="I38">
-        <v>1.415045324648525</v>
+        <v>1.415309301725443</v>
       </c>
     </row>
     <row r="39">
@@ -1643,10 +1643,10 @@
         <v>0</v>
       </c>
       <c r="E39">
-        <v>3.532145216423655</v>
+        <v>3.532122308897292</v>
       </c>
       <c r="F39">
-        <v>2.29567798826701</v>
+        <v>2.295420514539871</v>
       </c>
       <c r="G39">
         <v>0.1830775014705948</v>
@@ -1655,7 +1655,7 @@
         <v>0.4338389778553179</v>
       </c>
       <c r="I39">
-        <v>2.915228737097742</v>
+        <v>2.915205829571379</v>
       </c>
     </row>
     <row r="40">
@@ -1676,10 +1676,10 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>2.86395089891158</v>
+        <v>2.864287839047667</v>
       </c>
       <c r="F40">
-        <v>2.360576900522222</v>
+        <v>2.360466080986052</v>
       </c>
       <c r="G40">
         <v>1.644181498240886</v>
@@ -1688,7 +1688,7 @@
         <v>-0.7074856204578588</v>
       </c>
       <c r="I40">
-        <v>1.927255021128552</v>
+        <v>1.92759196126464</v>
       </c>
     </row>
     <row r="41">
@@ -1709,10 +1709,10 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>2.739523506820381</v>
+        <v>2.739702111884473</v>
       </c>
       <c r="F41">
-        <v>2.692089184251138</v>
+        <v>2.692278337938821</v>
       </c>
       <c r="G41">
         <v>0.4214418425158024</v>
@@ -1721,7 +1721,7 @@
         <v>-0.44606518048123</v>
       </c>
       <c r="I41">
-        <v>2.764146844785808</v>
+        <v>2.764325449849901</v>
       </c>
     </row>
     <row r="42">
@@ -1742,10 +1742,10 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>2.255680791332724</v>
+        <v>2.255849807384959</v>
       </c>
       <c r="F42">
-        <v>2.847825103372085</v>
+        <v>2.847990516803597</v>
       </c>
       <c r="G42">
         <v>0.6290059163210516</v>
@@ -1754,7 +1754,7 @@
         <v>-0.7144042446540373</v>
       </c>
       <c r="I42">
-        <v>2.34107911966571</v>
+        <v>2.341248135717945</v>
       </c>
     </row>
     <row r="43">
@@ -1775,10 +1775,10 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>1.494787064688244</v>
+        <v>1.495647569594783</v>
       </c>
       <c r="F43">
-        <v>2.338485565438233</v>
+        <v>2.33887183197797</v>
       </c>
       <c r="G43">
         <v>0.4901069572014474</v>
@@ -1787,7 +1787,7 @@
         <v>-1.063597864520708</v>
       </c>
       <c r="I43">
-        <v>2.068277972007504</v>
+        <v>2.069138476914044</v>
       </c>
     </row>
     <row r="44">
@@ -1808,10 +1808,10 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>1.197042502772424</v>
+        <v>1.196798063428107</v>
       </c>
       <c r="F44">
-        <v>1.921758466403444</v>
+        <v>1.92199938807308</v>
       </c>
       <c r="G44">
         <v>0.4203095613777605</v>
@@ -1820,7 +1820,7 @@
         <v>-0.37639879104271</v>
       </c>
       <c r="I44">
-        <v>1.153131732437373</v>
+        <v>1.152887293093057</v>
       </c>
     </row>
     <row r="45">
@@ -1841,10 +1841,10 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>0.1913936891530983</v>
+        <v>0.1911591396440102</v>
       </c>
       <c r="F45">
-        <v>1.284726011986623</v>
+        <v>1.284863645012964</v>
       </c>
       <c r="G45">
         <v>0.08455124436341505</v>
@@ -1853,7 +1853,7 @@
         <v>-0.9266923783968273</v>
       </c>
       <c r="I45">
-        <v>1.033534823186511</v>
+        <v>1.033300273677422</v>
       </c>
     </row>
     <row r="46">
@@ -1874,10 +1874,10 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <v>0.2280491170529774</v>
+        <v>0.2279892483689395</v>
       </c>
       <c r="F46">
-        <v>0.7778180934166865</v>
+        <v>0.7778985052589592</v>
       </c>
       <c r="G46">
         <v>-0.7063634794243945</v>
@@ -1886,7 +1886,7 @@
         <v>-0.08829624979960171</v>
       </c>
       <c r="I46">
-        <v>1.022708846276974</v>
+        <v>1.022648977592936</v>
       </c>
     </row>
     <row r="47">
@@ -1907,10 +1907,10 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>-1.43555459036326</v>
+        <v>-1.43528819058441</v>
       </c>
       <c r="F47">
-        <v>0.04523267965381062</v>
+        <v>0.04516456521416112</v>
       </c>
       <c r="G47">
         <v>-0.7791842320308732</v>
@@ -1919,7 +1919,7 @@
         <v>-0.5207276274948131</v>
       </c>
       <c r="I47">
-        <v>-0.1356427308375739</v>
+        <v>-0.1353763310587236</v>
       </c>
     </row>
     <row r="48">
@@ -1940,10 +1940,10 @@
         <v>0</v>
       </c>
       <c r="E48">
-        <v>-1.317036575972883</v>
+        <v>-1.317189124701745</v>
       </c>
       <c r="F48">
-        <v>-0.5832870900325162</v>
+        <v>-0.5833322318183018</v>
       </c>
       <c r="G48">
         <v>-0.1791826590862452</v>
@@ -1952,7 +1952,7 @@
         <v>-0.6686679888322142</v>
       </c>
       <c r="I48">
-        <v>-0.4691859280544238</v>
+        <v>-0.4693384767832854</v>
       </c>
     </row>
     <row r="49">
@@ -1973,10 +1973,10 @@
         <v>0</v>
       </c>
       <c r="E49">
-        <v>-2.163708922374684</v>
+        <v>-2.162992892311451</v>
       </c>
       <c r="F49">
-        <v>-1.172062742914462</v>
+        <v>-1.171870239807167</v>
       </c>
       <c r="G49">
         <v>-1.410076980392139</v>
@@ -1985,7 +1985,7 @@
         <v>-0.05152418484441068</v>
       </c>
       <c r="I49">
-        <v>-0.702107757138134</v>
+        <v>-0.7013917270749013</v>
       </c>
     </row>
     <row r="50">
@@ -2006,10 +2006,10 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>-1.085197855429417</v>
+        <v>-1.084930329632481</v>
       </c>
       <c r="F50">
-        <v>-1.500374486035061</v>
+        <v>-1.500100134307522</v>
       </c>
       <c r="G50">
         <v>-0.2105533183890024</v>
@@ -2018,7 +2018,7 @@
         <v>-0.1404336047976929</v>
       </c>
       <c r="I50">
-        <v>-0.7342109322427215</v>
+        <v>-0.7339434064457862</v>
       </c>
     </row>
     <row r="51">
@@ -2039,10 +2039,10 @@
         <v>0</v>
       </c>
       <c r="E51">
-        <v>-1.457193229872469</v>
+        <v>-1.457288912263728</v>
       </c>
       <c r="F51">
-        <v>-1.505784145912363</v>
+        <v>-1.505600314727352</v>
       </c>
       <c r="G51">
         <v>-0.3909270564522251</v>
@@ -2051,7 +2051,7 @@
         <v>-0.2560200781047454</v>
       </c>
       <c r="I51">
-        <v>-0.8102460953154985</v>
+        <v>-0.8103417777067574</v>
       </c>
     </row>
     <row r="52">
@@ -2072,10 +2072,10 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>-1.283561786197312</v>
+        <v>-1.284356325970676</v>
       </c>
       <c r="F52">
-        <v>-1.49741544846847</v>
+        <v>-1.497392115044585</v>
       </c>
       <c r="G52">
         <v>-0.6442132037942118</v>
@@ -2084,7 +2084,7 @@
         <v>-0.06640099407624728</v>
       </c>
       <c r="I52">
-        <v>-0.5729475883268532</v>
+        <v>-0.5737421281002171</v>
       </c>
     </row>
     <row r="53">
@@ -2105,10 +2105,10 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>-0.8579113804721512</v>
+        <v>-0.8583302477527929</v>
       </c>
       <c r="F53">
-        <v>-1.170966062992837</v>
+        <v>-1.17122645390492</v>
       </c>
       <c r="G53">
         <v>-0.07052941796100387</v>
@@ -2117,7 +2117,7 @@
         <v>-0.3554763575157842</v>
       </c>
       <c r="I53">
-        <v>-0.4319056049953631</v>
+        <v>-0.4323244722760048</v>
       </c>
     </row>
     <row r="54">
@@ -2138,10 +2138,10 @@
         <v>0</v>
       </c>
       <c r="E54">
-        <v>-1.56608131674303</v>
+        <v>-1.565634900165805</v>
       </c>
       <c r="F54">
-        <v>-1.29118692832124</v>
+        <v>-1.291402596538251</v>
       </c>
       <c r="G54">
         <v>-0.8865916234440627</v>
@@ -2150,7 +2150,7 @@
         <v>-0.1832364051070537</v>
       </c>
       <c r="I54">
-        <v>-0.4962532881919139</v>
+        <v>-0.4958068716146886</v>
       </c>
     </row>
     <row r="55">
@@ -2171,10 +2171,10 @@
         <v>0</v>
       </c>
       <c r="E55">
-        <v>-1.783417405602018</v>
+        <v>-1.783417127555434</v>
       </c>
       <c r="F55">
-        <v>-1.372742972253627</v>
+        <v>-1.372934650361178</v>
       </c>
       <c r="G55">
         <v>-1.047790882965999</v>
@@ -2183,7 +2183,7 @@
         <v>0.04953696020514492</v>
       </c>
       <c r="I55">
-        <v>-0.7851634828411646</v>
+        <v>-0.78516320479458</v>
       </c>
     </row>
     <row r="56">
@@ -2204,10 +2204,10 @@
         <v>0</v>
       </c>
       <c r="E56">
-        <v>-1.295826022465722</v>
+        <v>-1.295427428140189</v>
       </c>
       <c r="F56">
-        <v>-1.37580903132073</v>
+        <v>-1.375702425903556</v>
       </c>
       <c r="G56">
         <v>-0.3471829962638515</v>
@@ -2216,7 +2216,7 @@
         <v>-0.0966042891959619</v>
       </c>
       <c r="I56">
-        <v>-0.8520387370059082</v>
+        <v>-0.8516401426803758</v>
       </c>
     </row>
     <row r="57">
@@ -2237,10 +2237,10 @@
         <v>0</v>
       </c>
       <c r="E57">
-        <v>-1.152891776480925</v>
+        <v>-1.152610993212792</v>
       </c>
       <c r="F57">
-        <v>-1.449554130322923</v>
+        <v>-1.449272612268556</v>
       </c>
       <c r="G57">
         <v>-0.6132388212289077</v>
@@ -2249,7 +2249,7 @@
         <v>-0.1028635192602457</v>
       </c>
       <c r="I57">
-        <v>-0.4367894359917712</v>
+        <v>-0.4365086527236389</v>
       </c>
     </row>
     <row r="58">
@@ -2270,10 +2270,10 @@
         <v>0</v>
       </c>
       <c r="E58">
-        <v>-1.384154271490635</v>
+        <v>-1.384226526985612</v>
       </c>
       <c r="F58">
-        <v>-1.404072369009824</v>
+        <v>-1.403920518973508</v>
       </c>
       <c r="G58">
         <v>-0.9172888700772799</v>
@@ -2282,7 +2282,7 @@
         <v>0.01540737794330799</v>
       </c>
       <c r="I58">
-        <v>-0.4822727793566633</v>
+        <v>-0.4823450348516403</v>
       </c>
     </row>
     <row r="59">
@@ -2303,10 +2303,10 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>-1.297127733297142</v>
+        <v>-1.297272162778938</v>
       </c>
       <c r="F59">
-        <v>-1.282499950933605</v>
+        <v>-1.282384277779384</v>
       </c>
       <c r="G59">
         <v>-0.2587432465973415</v>
@@ -2315,7 +2315,7 @@
         <v>-0.3629080917018036</v>
       </c>
       <c r="I59">
-        <v>-0.6754763949979967</v>
+        <v>-0.6756208244797927</v>
       </c>
     </row>
     <row r="60">
@@ -2336,10 +2336,10 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>-0.7502484479585195</v>
+        <v>-0.7507150353225633</v>
       </c>
       <c r="F60">
-        <v>-1.146105557306805</v>
+        <v>-1.146206179574977</v>
       </c>
       <c r="G60">
         <v>-0.09302646274323331</v>
@@ -2348,7 +2348,7 @@
         <v>-0.1298910337959616</v>
       </c>
       <c r="I60">
-        <v>-0.5273309514193246</v>
+        <v>-0.5277975387833684</v>
       </c>
     </row>
     <row r="61">
@@ -2369,10 +2369,10 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <v>-0.1723529222894641</v>
+        <v>-0.1726286086756727</v>
       </c>
       <c r="F61">
-        <v>-0.9009708437589395</v>
+        <v>-0.9012105834406974</v>
       </c>
       <c r="G61">
         <v>0.03469619020211948</v>
@@ -2381,7 +2381,7 @@
         <v>0.1381184495505191</v>
       </c>
       <c r="I61">
-        <v>-0.3451675620421027</v>
+        <v>-0.3454432484283113</v>
       </c>
     </row>
     <row r="62">
@@ -2402,10 +2402,10 @@
         <v>0</v>
       </c>
       <c r="E62">
-        <v>-0.5414991552362339</v>
+        <v>-0.5422171705718358</v>
       </c>
       <c r="F62">
-        <v>-0.6903070646953393</v>
+        <v>-0.6907082443372532</v>
       </c>
       <c r="G62">
         <v>-0.8456653475137066</v>
@@ -2414,7 +2414,7 @@
         <v>0.4977560396995079</v>
       </c>
       <c r="I62">
-        <v>-0.1935898474220353</v>
+        <v>-0.1943078627576371</v>
       </c>
     </row>
     <row r="63">
@@ -2435,10 +2435,10 @@
         <v>0</v>
       </c>
       <c r="E63">
-        <v>0.07521201813555149</v>
+        <v>0.07508084834374588</v>
       </c>
       <c r="F63">
-        <v>-0.347222126837166</v>
+        <v>-0.3476199915565823</v>
       </c>
       <c r="G63">
         <v>0.0488266565076218</v>
@@ -2447,7 +2447,7 @@
         <v>0.00794499122983091</v>
       </c>
       <c r="I63">
-        <v>0.01844037039809878</v>
+        <v>0.01830920060629317</v>
       </c>
     </row>
     <row r="64">
@@ -2468,10 +2468,10 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>0.286690415375635</v>
+        <v>0.2871956342159526</v>
       </c>
       <c r="F64">
-        <v>-0.08798741100362742</v>
+        <v>-0.08814232417195333</v>
       </c>
       <c r="G64">
         <v>-0.07135988355089964</v>
@@ -2480,7 +2480,7 @@
         <v>0.3696321006761685</v>
       </c>
       <c r="I64">
-        <v>-0.01158180174963387</v>
+        <v>-0.01107658290931631</v>
       </c>
     </row>
     <row r="65">
@@ -2501,10 +2501,10 @@
         <v>0</v>
       </c>
       <c r="E65">
-        <v>0.03462809556592961</v>
+        <v>0.0348932722193499</v>
       </c>
       <c r="F65">
-        <v>-0.036242156539779</v>
+        <v>-0.03626185394819768</v>
       </c>
       <c r="G65">
         <v>-0.04123200610439566</v>
@@ -2513,7 +2513,7 @@
         <v>0.05673608506707493</v>
       </c>
       <c r="I65">
-        <v>0.01912401660325034</v>
+        <v>0.01938919325667063</v>
       </c>
     </row>
     <row r="66">
@@ -2534,10 +2534,10 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>-0.1011811643181902</v>
+        <v>-0.1005819750487675</v>
       </c>
       <c r="F66">
-        <v>0.07383734118973195</v>
+        <v>0.0741469449325694</v>
       </c>
       <c r="G66">
         <v>0.1305714754136182</v>
@@ -2546,7 +2546,7 @@
         <v>-0.1739916507745391</v>
       </c>
       <c r="I66">
-        <v>-0.05776098895726919</v>
+        <v>-0.05716179968784655</v>
       </c>
     </row>
     <row r="67">
@@ -2567,10 +2567,10 @@
         <v>0</v>
       </c>
       <c r="E67">
-        <v>0.3179058919803286</v>
+        <v>0.317607350645855</v>
       </c>
       <c r="F67">
-        <v>0.1345108096509262</v>
+        <v>0.1347785705080967</v>
       </c>
       <c r="G67">
         <v>-0.0095204543947928</v>
@@ -2579,7 +2579,7 @@
         <v>0.3618699123118419</v>
       </c>
       <c r="I67">
-        <v>-0.0344435659367205</v>
+        <v>-0.03474210727119406</v>
       </c>
     </row>
     <row r="68">
@@ -2600,10 +2600,10 @@
         <v>0</v>
       </c>
       <c r="E68">
-        <v>-0.4745098658630824</v>
+        <v>-0.4746798065130151</v>
       </c>
       <c r="F68">
-        <v>-0.0557892606587531</v>
+        <v>-0.05569028967414523</v>
       </c>
       <c r="G68">
         <v>-0.2028730263807215</v>
@@ -2612,7 +2612,7 @@
         <v>-0.1980140598340873</v>
       </c>
       <c r="I68">
-        <v>-0.0736227796482735</v>
+        <v>-0.07379272029820626</v>
       </c>
     </row>
     <row r="69">
@@ -2633,10 +2633,10 @@
         <v>0</v>
       </c>
       <c r="E69">
-        <v>-0.09254941770088418</v>
+        <v>-0.09238412162976098</v>
       </c>
       <c r="F69">
-        <v>-0.08758363897545654</v>
+        <v>-0.08750963813642296</v>
       </c>
       <c r="G69">
         <v>-0.0594327661714883</v>
@@ -2645,7 +2645,7 @@
         <v>0.1054090751596382</v>
       </c>
       <c r="I69">
-        <v>-0.1385257266890341</v>
+        <v>-0.1383604306179109</v>
       </c>
     </row>
     <row r="70">
@@ -2666,19 +2666,19 @@
         <v>0</v>
       </c>
       <c r="E70">
-        <v>-0.1993498198189684</v>
+        <v>-0.1990579218844226</v>
       </c>
       <c r="F70">
-        <v>-0.1121258028506511</v>
+        <v>-0.1121286248453367</v>
       </c>
       <c r="G70">
-        <v>-0.1469082386613493</v>
+        <v>-0.1469082386613492</v>
       </c>
       <c r="H70">
         <v>0.05240041216595906</v>
       </c>
       <c r="I70">
-        <v>-0.1048419933235782</v>
+        <v>-0.1045500953890324</v>
       </c>
     </row>
     <row r="71">
@@ -2699,10 +2699,10 @@
         <v>0</v>
       </c>
       <c r="E71">
-        <v>-0.2105616900593215</v>
+        <v>-0.2103550967322966</v>
       </c>
       <c r="F71">
-        <v>-0.2442426983605636</v>
+        <v>-0.2441192366898746</v>
       </c>
       <c r="G71">
         <v>-0.2842812308453224</v>
@@ -2711,7 +2711,7 @@
         <v>0.01102558298453079</v>
       </c>
       <c r="I71">
-        <v>0.0626939578014702</v>
+        <v>0.06290055112849507</v>
       </c>
     </row>
     <row r="72">
@@ -2732,10 +2732,10 @@
         <v>0</v>
       </c>
       <c r="E72">
-        <v>0.07546623696688659</v>
+        <v>0.07533844586083796</v>
       </c>
       <c r="F72">
-        <v>-0.1067486726530714</v>
+        <v>-0.1066146735964113</v>
       </c>
       <c r="G72">
         <v>0.1101517719974749</v>
@@ -2744,7 +2744,7 @@
         <v>-0.1229138139409729</v>
       </c>
       <c r="I72">
-        <v>0.08822827891038453</v>
+        <v>0.08810048780433589</v>
       </c>
     </row>
     <row r="73">
@@ -2765,10 +2765,10 @@
         <v>0</v>
       </c>
       <c r="E73">
-        <v>-0.2288536337787813</v>
+        <v>-0.2287256002259627</v>
       </c>
       <c r="F73">
-        <v>-0.1408247266725457</v>
+        <v>-0.1407000432454618</v>
       </c>
       <c r="G73">
         <v>-0.3642509696606954</v>
@@ -2777,7 +2777,7 @@
         <v>0.1086193414943325</v>
       </c>
       <c r="I73">
-        <v>0.02677799438758162</v>
+        <v>0.02690602794040024</v>
       </c>
     </row>
     <row r="74">
@@ -2798,10 +2798,10 @@
         <v>0</v>
       </c>
       <c r="E74">
-        <v>0.03946169552298146</v>
+        <v>0.03959594375674771</v>
       </c>
       <c r="F74">
-        <v>-0.0811218478370582</v>
+        <v>-0.0810365768351692</v>
       </c>
       <c r="G74">
         <v>0.2237569875946429</v>
@@ -2810,7 +2810,7 @@
         <v>-0.02712450934502616</v>
       </c>
       <c r="I74">
-        <v>-0.1571707827266353</v>
+        <v>-0.157036534492869</v>
       </c>
     </row>
     <row r="75">
@@ -2831,10 +2831,10 @@
         <v>0</v>
       </c>
       <c r="E75">
-        <v>0.01842065120159704</v>
+        <v>0.0181712003829638</v>
       </c>
       <c r="F75">
-        <v>-0.02387626252182858</v>
+        <v>-0.02390500255635411</v>
       </c>
       <c r="G75">
         <v>-0.01311419685234618</v>
@@ -2843,7 +2843,7 @@
         <v>-0.03836760891619392</v>
       </c>
       <c r="I75">
-        <v>0.06990245697013714</v>
+        <v>0.0696530061515039</v>
       </c>
     </row>
     <row r="76">
@@ -2864,10 +2864,10 @@
         <v>0</v>
       </c>
       <c r="E76">
-        <v>0.4273326313133025</v>
+        <v>0.4273310033908086</v>
       </c>
       <c r="F76">
-        <v>0.06409033606477539</v>
+        <v>0.06409313682613854</v>
       </c>
       <c r="G76">
         <v>0.007741184328022455</v>
@@ -2876,7 +2876,7 @@
         <v>0.1820306418640798</v>
       </c>
       <c r="I76">
-        <v>0.2375608051212002</v>
+        <v>0.2375591771987063</v>
       </c>
     </row>
     <row r="77">
@@ -2897,10 +2897,10 @@
         <v>0</v>
       </c>
       <c r="E77">
-        <v>0.1652983376755857</v>
+        <v>0.1656468001724334</v>
       </c>
       <c r="F77">
-        <v>0.1626283289283672</v>
+        <v>0.1626862369257376</v>
       </c>
       <c r="G77">
         <v>0.1832164717785813</v>
@@ -2909,7 +2909,7 @@
         <v>-0.0655278868595966</v>
       </c>
       <c r="I77">
-        <v>0.04760975275660094</v>
+        <v>0.04795821525344868</v>
       </c>
     </row>
     <row r="78">
@@ -2930,10 +2930,10 @@
         <v>0</v>
       </c>
       <c r="E78">
-        <v>-0.4280824757189858</v>
+        <v>-0.4280410883731992</v>
       </c>
       <c r="F78">
-        <v>0.04574228611787533</v>
+        <v>0.04577697889325084</v>
       </c>
       <c r="G78">
         <v>-0.0319629231639949</v>
@@ -2942,7 +2942,7 @@
         <v>-0.4472970132207758</v>
       </c>
       <c r="I78">
-        <v>0.05117746066578486</v>
+        <v>0.05121884801157155</v>
       </c>
     </row>
     <row r="79">
@@ -2963,10 +2963,10 @@
         <v>0</v>
       </c>
       <c r="E79">
-        <v>0.211407231042728</v>
+        <v>0.2109907177307189</v>
       </c>
       <c r="F79">
-        <v>0.09398893107815808</v>
+        <v>0.09398185823018962</v>
       </c>
       <c r="G79">
         <v>-0.1261415442716636</v>
@@ -2975,7 +2975,7 @@
         <v>0.234931818107759</v>
       </c>
       <c r="I79">
-        <v>0.1026169572066326</v>
+        <v>0.1022004438946236</v>
       </c>
     </row>
     <row r="80">
@@ -2996,10 +2996,10 @@
         <v>0</v>
       </c>
       <c r="E80">
-        <v>0.6139640220240625</v>
+        <v>0.6139051435579954</v>
       </c>
       <c r="F80">
-        <v>0.1406467787558481</v>
+        <v>0.1406253932719863</v>
       </c>
       <c r="G80">
         <v>0.43627845986265</v>
@@ -3008,7 +3008,7 @@
         <v>0.1023935315640581</v>
       </c>
       <c r="I80">
-        <v>0.07529203059735448</v>
+        <v>0.07523315213128735</v>
       </c>
     </row>
     <row r="81">
@@ -3029,10 +3029,10 @@
         <v>0</v>
       </c>
       <c r="E81">
-        <v>0.4001201119220791</v>
+        <v>0.4001838849401698</v>
       </c>
       <c r="F81">
-        <v>0.1993522223174715</v>
+        <v>0.1992596644639204</v>
       </c>
       <c r="G81">
         <v>0.1698509031992773</v>
@@ -3041,7 +3041,7 @@
         <v>-0.117298132789972</v>
       </c>
       <c r="I81">
-        <v>0.3475673415127739</v>
+        <v>0.3476311145308645</v>
       </c>
     </row>
     <row r="82">
@@ -3062,10 +3062,10 @@
         <v>0</v>
       </c>
       <c r="E82">
-        <v>0.4816080942708365</v>
+        <v>0.4806702503234167</v>
       </c>
       <c r="F82">
-        <v>0.4267748648149271</v>
+        <v>0.4264374991380743</v>
       </c>
       <c r="G82">
         <v>0.3437108920115783</v>
@@ -3074,7 +3074,7 @@
         <v>-0.2466962259924505</v>
       </c>
       <c r="I82">
-        <v>0.3845934282517087</v>
+        <v>0.3836555843042889</v>
       </c>
     </row>
     <row r="83">
@@ -3095,10 +3095,10 @@
         <v>0</v>
       </c>
       <c r="E83">
-        <v>0.08506766165855074</v>
+        <v>0.08512296786821864</v>
       </c>
       <c r="F83">
-        <v>0.3951899724688828</v>
+        <v>0.3949705616724493</v>
       </c>
       <c r="G83">
         <v>-0.02351814460598127</v>
@@ -3107,7 +3107,7 @@
         <v>-0.07249663819006502</v>
       </c>
       <c r="I83">
-        <v>0.181082444454597</v>
+        <v>0.1811377506642649</v>
       </c>
     </row>
     <row r="84">
@@ -3128,19 +3128,19 @@
         <v>0</v>
       </c>
       <c r="E84">
-        <v>14.31048153771793</v>
+        <v>14.30995993990337</v>
       </c>
       <c r="F84">
-        <v>3.819319351392349</v>
+        <v>3.818984260758794</v>
       </c>
       <c r="G84">
-        <v>2.31906979058428</v>
+        <v>13.5431724569603</v>
       </c>
       <c r="H84">
-        <v>-2.205623585545855</v>
+        <v>-13.42972625192188</v>
       </c>
       <c r="I84">
-        <v>14.1970353326795</v>
+        <v>14.19651373486495</v>
       </c>
     </row>
     <row r="85">
@@ -3161,19 +3161,19 @@
         <v>0</v>
       </c>
       <c r="E85">
-        <v>3.778604641253938</v>
+        <v>3.778452450136442</v>
       </c>
       <c r="F85">
-        <v>4.663940483725313</v>
+        <v>4.663551402057863</v>
       </c>
       <c r="G85">
-        <v>-0.5073236800666964</v>
+        <v>-14.00135327692795</v>
       </c>
       <c r="H85">
-        <v>-0.6537520414966955</v>
+        <v>12.84027755536455</v>
       </c>
       <c r="I85">
-        <v>4.93968036281733</v>
+        <v>4.939528171699834</v>
       </c>
     </row>
     <row r="86">
@@ -3191,19 +3191,19 @@
         <v>1</v>
       </c>
       <c r="E86">
-        <v>-3.065722918839948</v>
+        <v>-0.7484702393197009</v>
       </c>
       <c r="F86">
-        <v>3.777107730447617</v>
+        <v>4.356266279647083</v>
       </c>
       <c r="G86">
-        <v>0.20079346384812</v>
+        <v>-0.2556728698451678</v>
       </c>
       <c r="H86">
-        <v>-0.3682804751894168</v>
+        <v>0.08818585850387101</v>
       </c>
       <c r="I86">
-        <v>-2.898235907498652</v>
+        <v>-0.5809832279784041</v>
       </c>
     </row>
     <row r="87">
@@ -3221,19 +3221,19 @@
         <v>1</v>
       </c>
       <c r="E87">
-        <v>-1.61870889521577</v>
+        <v>0.3091232364041231</v>
       </c>
       <c r="F87">
-        <v>3.351163591229037</v>
+        <v>4.412266346781059</v>
       </c>
       <c r="G87">
-        <v>-0.4326739975981833</v>
+        <v>-0.4125729743443741</v>
       </c>
       <c r="H87">
-        <v>0.1636240993943216</v>
+        <v>0.1435230761405124</v>
       </c>
       <c r="I87">
-        <v>-1.349658997011909</v>
+        <v>0.5781731346079848</v>
       </c>
     </row>
     <row r="88">
@@ -3251,19 +3251,19 @@
         <v>1</v>
       </c>
       <c r="E88">
-        <v>-2.775808604688196</v>
+        <v>-1.21536068712779</v>
       </c>
       <c r="F88">
-        <v>-0.9204089443724932</v>
+        <v>0.5309361900232683</v>
       </c>
       <c r="G88">
-        <v>-0.6709843528819649</v>
+        <v>-0.4413344611392941</v>
       </c>
       <c r="H88">
-        <v>0.2530881761718929</v>
+        <v>0.02343828442922213</v>
       </c>
       <c r="I88">
-        <v>-2.357912427978123</v>
+        <v>-0.7974645104177175</v>
       </c>
     </row>
     <row r="89">
@@ -3281,19 +3281,19 @@
         <v>1</v>
       </c>
       <c r="E89">
-        <v>-3.072587706092993</v>
+        <v>-1.516292281821854</v>
       </c>
       <c r="F89">
-        <v>-2.633207031209226</v>
+        <v>-0.7927499929663057</v>
       </c>
       <c r="G89">
-        <v>-0.1175485603499245</v>
+        <v>-0.388192966708367</v>
       </c>
       <c r="H89">
-        <v>-0.1587125613039996</v>
+        <v>0.1119318450544428</v>
       </c>
       <c r="I89">
-        <v>-2.796326584439069</v>
+        <v>-1.24003116016793</v>
       </c>
     </row>
     <row r="90">
@@ -3311,19 +3311,19 @@
         <v>1</v>
       </c>
       <c r="E90">
-        <v>-2.176961391123295</v>
+        <v>-1.928824926219217</v>
       </c>
       <c r="F90">
-        <v>-2.411016649280063</v>
+        <v>-1.087838664691184</v>
       </c>
       <c r="G90">
-        <v>-0.1571464430805447</v>
+        <v>0.1340162546123547</v>
       </c>
       <c r="H90">
-        <v>0.03537450785307342</v>
+        <v>-0.255788189839826</v>
       </c>
       <c r="I90">
-        <v>-2.055189455895823</v>
+        <v>-1.807052990991745</v>
       </c>
     </row>
     <row r="91">
@@ -3341,19 +3341,19 @@
         <v>1</v>
       </c>
       <c r="E91">
-        <v>-1.044746300494312</v>
+        <v>-0.423142510523442</v>
       </c>
       <c r="F91">
-        <v>-2.267526000599698</v>
+        <v>-1.270905101423076</v>
       </c>
       <c r="G91">
-        <v>-0.1481602573195862</v>
+        <v>0.1485459750704547</v>
       </c>
       <c r="H91">
-        <v>0.09121439988336716</v>
+        <v>-0.2054918325066737</v>
       </c>
       <c r="I91">
-        <v>-0.9878004430580928</v>
+        <v>-0.3661966530872229</v>
       </c>
     </row>
     <row r="92">
@@ -3371,19 +3371,19 @@
         <v>1</v>
       </c>
       <c r="E92">
-        <v>-1.939381019320358</v>
+        <v>-1.008438099083801</v>
       </c>
       <c r="F92">
-        <v>-2.058419104257739</v>
+        <v>-1.219174454412078</v>
       </c>
       <c r="G92">
-        <v>-0.04498005828145774</v>
+        <v>0.1434629256086545</v>
       </c>
       <c r="H92">
-        <v>-0.0124802458074785</v>
+        <v>-0.2009232296975907</v>
       </c>
       <c r="I92">
-        <v>-1.881920715231421</v>
+        <v>-0.9509777949948648</v>
       </c>
     </row>
     <row r="93">
@@ -3401,19 +3401,19 @@
         <v>1</v>
       </c>
       <c r="E93">
-        <v>-0.5893346741417274</v>
+        <v>0.3657705776902921</v>
       </c>
       <c r="F93">
-        <v>-1.437605846269922</v>
+        <v>-0.7486587395340417</v>
       </c>
       <c r="G93">
-        <v>-0.02176260558866694</v>
+        <v>0.1721890068410809</v>
       </c>
       <c r="H93">
-        <v>-0.07385186464188666</v>
+        <v>-0.2678034770716344</v>
       </c>
       <c r="I93">
-        <v>-0.4937202039111737</v>
+        <v>0.4613850479208457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>